<commit_message>
changed name of constraint results summary file and completed analysis of several constrained games
</commit_message>
<xml_diff>
--- a/Domination/game-logs/constricted-play-samples/ConstrainedPSR.xlsx
+++ b/Domination/game-logs/constricted-play-samples/ConstrainedPSR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="431" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Samples Collected</t>
   </si>
@@ -31,9 +31,15 @@
     <t>Percentage</t>
   </si>
   <si>
+    <t>Done con 3,4,5,6,8</t>
+  </si>
+  <si>
     <t>Constrained P Accuracy Measures</t>
   </si>
   <si>
+    <t>Marks are made for the highest probability among explanations for a player</t>
+  </si>
+  <si>
     <t>Percentage Accuracy</t>
   </si>
   <si>
@@ -58,10 +64,10 @@
     <t>I P - 3 C</t>
   </si>
   <si>
-    <t>In P L– 2 con</t>
-  </si>
-  <si>
-    <t>In P W – 3 C</t>
+    <t>In P – 2 C</t>
+  </si>
+  <si>
+    <t>In P – 3 C</t>
   </si>
   <si>
     <r>
@@ -85,6 +91,7 @@
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -93,12 +100,16 @@
     </r>
   </si>
   <si>
+    <t>Wrong</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">C</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -107,12 +118,16 @@
     </r>
   </si>
   <si>
+    <t>Spent most of game attacking a single continent Fred Con-4</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">2C</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -121,12 +136,16 @@
     </r>
   </si>
   <si>
+    <t>Bob – con 5</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">3C</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -135,12 +154,16 @@
     </r>
   </si>
   <si>
+    <t>the grapes – con 5</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">W</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -150,11 +173,27 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">L</t>
+      <t xml:space="preserve">Border line </t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">new player – con 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">L</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -164,11 +203,27 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">In</t>
+      <t xml:space="preserve">Border line </t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">fred con 8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="00000000"/>
         <sz val="11"/>
@@ -177,10 +232,50 @@
     </r>
   </si>
   <si>
+    <t>Inconclusive</t>
+  </si>
+  <si>
+    <t>s0914007 Con 4</t>
+  </si>
+  <si>
+    <t>ted con 4</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Missed large amount of actions at end due to sampling at end of turn only winner inconclusive! </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">Mr abc con 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">yura con 5 </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="true"/>
+        <color rgb="00000000"/>
+        <sz val="11"/>
+      </rPr>
+      <t xml:space="preserve">did not get a chance to attack last continent</t>
+    </r>
+  </si>
+  <si>
     <t>C P W</t>
   </si>
   <si>
-    <t>C P L </t>
+    <t>C P L</t>
   </si>
   <si>
     <t>I P W</t>
@@ -199,12 +294,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="0.00%" numFmtId="166"/>
+    <numFmt formatCode="0.00%" numFmtId="165"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
@@ -232,19 +326,6 @@
       <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color rgb="00000000"/>
       <sz val="11"/>
     </font>
@@ -291,12 +372,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -314,34 +394,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T36"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100">
-      <selection activeCell="F9" activeCellId="0" pane="topLeft" sqref="F9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100">
+      <selection activeCell="F14" activeCellId="0" pane="topLeft" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.89803921568628"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.4862745098039"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.34117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.93725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.2"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.73725490196078"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.74901960784314"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.89803921568628"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.2"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.16078431372549"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.2078431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.85882352941176"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.4705882352941"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="3.56470588235294"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.4705882352941"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="14.3254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.478431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="4.91764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6078431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="5.96470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.22745098039216"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.75686274509804"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.77647058823529"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="4.91764705882353"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="7.22745098039216"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.18039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.87058823529412"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.3843137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="3.57647058823529"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.9529411764706"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="4.89803921568628"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="10.4705882352941"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -357,6 +439,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
       <c r="A2" s="0" t="n">
@@ -376,21 +461,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
       <c r="A3" s="0" t="n">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>100</v>
       </c>
       <c r="C3" s="2" t="n">
         <f aca="false">(B3-A3)</f>
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="D3" s="3" t="n">
         <f aca="false">(C3/B3)</f>
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
@@ -408,41 +493,45 @@
         <f aca="false">(C4/B4)</f>
         <v>0.448</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="8">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="U8" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="9">
       <c r="G9" s="3" t="n">
@@ -463,14 +552,21 @@
       <c r="Q9" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>16</v>
+      <c r="S9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="3"/>
+      <c r="V9" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="10">
       <c r="G10" s="3" t="n">
         <v>0.75</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I10" s="3" t="n">
         <v>0.6</v>
       </c>
@@ -486,14 +582,21 @@
       <c r="Q10" s="3" t="n">
         <v>0.75</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>17</v>
+      <c r="S10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="3"/>
+      <c r="V10" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="11">
       <c r="G11" s="3" t="n">
         <v>0.7</v>
       </c>
+      <c r="H11" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I11" s="3" t="n">
         <v>0.5</v>
       </c>
@@ -509,17 +612,27 @@
       <c r="Q11" s="3" t="n">
         <v>0.7</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>18</v>
+      <c r="S11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U11" s="3"/>
+      <c r="V11" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="12">
       <c r="G12" s="3" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I12" s="3" t="n">
         <v>0.4</v>
       </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K12" s="3" t="n">
         <v>0.6</v>
       </c>
@@ -532,13 +645,20 @@
       <c r="Q12" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="T12" s="4" t="s">
-        <v>19</v>
+      <c r="S12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="13">
       <c r="G13" s="3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>0.3</v>
@@ -555,17 +675,27 @@
       <c r="Q13" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="T13" s="4" t="s">
-        <v>20</v>
+      <c r="S13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="14">
       <c r="G14" s="3" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I14" s="3" t="n">
         <v>0.25</v>
       </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K14" s="3" t="n">
         <v>0.45</v>
       </c>
@@ -578,17 +708,27 @@
       <c r="Q14" s="3" t="n">
         <v>0.45</v>
       </c>
-      <c r="T14" s="4" t="s">
-        <v>21</v>
+      <c r="S14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U14" s="3"/>
+      <c r="V14" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="15">
       <c r="G15" s="3" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I15" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K15" s="3" t="n">
         <v>0.4</v>
       </c>
@@ -601,33 +741,51 @@
       <c r="Q15" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="T15" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="S15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U15" s="3"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="16">
       <c r="G16" s="3" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I16" s="3" t="n">
         <v>0.15</v>
       </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="K16" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="M16" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="N16" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="O16" s="3" t="n">
         <v>0.3</v>
       </c>
       <c r="Q16" s="3" t="n">
         <v>0.3</v>
       </c>
+      <c r="S16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="17">
       <c r="G17" s="3" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="I17" s="3" t="n">
         <v>0.1</v>
@@ -635,6 +793,9 @@
       <c r="K17" s="3" t="n">
         <v>0.25</v>
       </c>
+      <c r="L17" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="M17" s="3" t="n">
         <v>0.15</v>
       </c>
@@ -644,27 +805,52 @@
       <c r="Q17" s="3" t="n">
         <v>0.25</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="18">
+      <c r="S17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="18">
       <c r="G18" s="3" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K18" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="L18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="M18" s="3" t="n">
         <v>0.1</v>
       </c>
+      <c r="N18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="O18" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="P18" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q18" s="3" t="n">
         <v>0.2</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="19">
+      <c r="S18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="19">
       <c r="G19" s="3" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="K19" s="3" t="n">
         <v>0.1</v>
@@ -672,36 +858,71 @@
       <c r="O19" s="3" t="n">
         <v>0.15</v>
       </c>
+      <c r="P19" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q19" s="3" t="n">
         <v>0.15</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="20">
+      <c r="R19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="20">
+      <c r="G20" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="O20" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="Q20" s="3" t="n">
         <v>0.1</v>
       </c>
+      <c r="S20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="21">
+      <c r="G21" s="3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="22">
+      <c r="G22" s="3" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="24">
       <c r="G24" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="25">
@@ -728,8 +949,14 @@
       <c r="G26" s="3" t="n">
         <v>0.7</v>
       </c>
+      <c r="H26" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I26" s="3" t="n">
         <v>0.75</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K26" s="3" t="n">
         <v>0.7</v>
@@ -768,8 +995,14 @@
       <c r="G28" s="3" t="n">
         <v>0.45</v>
       </c>
+      <c r="H28" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I28" s="3" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K28" s="3" t="n">
         <v>0.45</v>
@@ -788,8 +1021,14 @@
       <c r="G29" s="3" t="n">
         <v>0.4</v>
       </c>
+      <c r="H29" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I29" s="3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="K29" s="3" t="n">
         <v>0.4</v>
@@ -809,7 +1048,10 @@
         <v>0.3</v>
       </c>
       <c r="I30" s="3" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K30" s="3" t="n">
         <v>0.3</v>
@@ -829,7 +1071,7 @@
         <v>0.25</v>
       </c>
       <c r="I31" s="3" t="n">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="K31" s="3" t="n">
         <v>0.25</v>
@@ -848,14 +1090,23 @@
       <c r="G32" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="H32" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="I32" s="3" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K32" s="3" t="n">
         <v>0.2</v>
       </c>
       <c r="M32" s="3" t="n">
         <v>0.25</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="O32" s="3" t="n">
         <v>0.3</v>
@@ -869,14 +1120,20 @@
         <v>0.1</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>0.25</v>
+        <v>0.35</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="K33" s="3" t="n">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="M33" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="N33" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="O33" s="3" t="n">
         <v>0.25</v>
       </c>
@@ -886,37 +1143,74 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="34">
       <c r="I34" s="3" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="K34" s="3" t="n">
+        <v>0.1</v>
       </c>
       <c r="M34" s="3" t="n">
         <v>0.1</v>
       </c>
+      <c r="N34" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="O34" s="3" t="n">
         <v>0.2</v>
       </c>
       <c r="Q34" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="R34" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="35">
       <c r="I35" s="3" t="n">
-        <v>0.1</v>
+        <v>0.25</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="O35" s="3" t="n">
         <v>0.15</v>
       </c>
+      <c r="P35" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="Q35" s="3" t="n">
         <v>0.15</v>
       </c>
+      <c r="R35" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="36">
+      <c r="I36" s="3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>2</v>
+      </c>
       <c r="O36" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="Q36" s="3" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="37">
+      <c r="I37" s="3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
+      <c r="I38" s="3" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -943,7 +1237,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -968,7 +1262,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.60392156862745"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>